<commit_message>
menu et sous menu Bail, niveau modifer bail terminer
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding\app\inf1163 projet\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF97513-F572-4A0D-8A5C-7F5FE248C3FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C0BF6A-BD4E-44AF-968F-1D1E339711F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20805" yWindow="1935" windowWidth="13995" windowHeight="13665" xr2:uid="{42D0C8F0-C429-4306-AA01-3F8905980968}"/>
+    <workbookView xWindow="-28365" yWindow="450" windowWidth="21165" windowHeight="13665" activeTab="2" xr2:uid="{42D0C8F0-C429-4306-AA01-3F8905980968}"/>
   </bookViews>
   <sheets>
     <sheet name="locataires" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="203">
   <si>
     <t>prénom</t>
   </si>
@@ -395,9 +395,6 @@
     <t>Kenya Schmitt</t>
   </si>
   <si>
-    <t>typeUnités</t>
-  </si>
-  <si>
     <t>locataire</t>
   </si>
   <si>
@@ -410,9 +407,6 @@
     <t>idAssurance</t>
   </si>
   <si>
-    <t>revouvelabilité</t>
-  </si>
-  <si>
     <t>remisage</t>
   </si>
   <si>
@@ -645,6 +639,15 @@
   </si>
   <si>
     <t>residentiel</t>
+  </si>
+  <si>
+    <t>idUnites</t>
+  </si>
+  <si>
+    <t>date entree</t>
+  </si>
+  <si>
+    <t>revouvelabiliter</t>
   </si>
 </sst>
 </file>
@@ -1030,7 +1033,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A6D0A01-9956-49E9-B0EE-E2DDB5E0B1CD}">
   <dimension ref="B2:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -1049,22 +1052,22 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E2" t="s">
         <v>1</v>
       </c>
       <c r="F2" t="s">
+        <v>192</v>
+      </c>
+      <c r="G2" t="s">
+        <v>193</v>
+      </c>
+      <c r="H2" t="s">
         <v>194</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>195</v>
-      </c>
-      <c r="H2" t="s">
-        <v>196</v>
-      </c>
-      <c r="I2" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="3" spans="2:9" ht="16.5" x14ac:dyDescent="0.25">
@@ -1100,7 +1103,7 @@
         <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F4" t="s">
         <v>48</v>
@@ -1109,7 +1112,7 @@
         <v>61</v>
       </c>
       <c r="H4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="I4">
         <v>657</v>
@@ -1157,7 +1160,7 @@
         <v>61</v>
       </c>
       <c r="H6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="I6">
         <v>787</v>
@@ -1181,7 +1184,7 @@
         <v>61</v>
       </c>
       <c r="H7" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="I7">
         <v>763</v>
@@ -1205,7 +1208,7 @@
         <v>61</v>
       </c>
       <c r="H8" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="I8">
         <v>682</v>
@@ -1301,7 +1304,7 @@
         <v>62</v>
       </c>
       <c r="H12" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="I12">
         <v>758</v>
@@ -1310,7 +1313,7 @@
     <row r="13" spans="2:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D13" t="s">
         <v>10</v>
@@ -1325,7 +1328,7 @@
         <v>62</v>
       </c>
       <c r="H13" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="I13">
         <v>718</v>
@@ -1349,7 +1352,7 @@
         <v>62</v>
       </c>
       <c r="H14" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="I14">
         <v>811</v>
@@ -1373,7 +1376,7 @@
         <v>62</v>
       </c>
       <c r="H15" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="I15">
         <v>692</v>
@@ -1388,7 +1391,7 @@
         <v>17</v>
       </c>
       <c r="E16" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F16" t="s">
         <v>59</v>
@@ -1421,7 +1424,7 @@
         <v>62</v>
       </c>
       <c r="H17" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="I17">
         <v>738</v>
@@ -1458,7 +1461,7 @@
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -1485,13 +1488,13 @@
         <v>68</v>
       </c>
       <c r="K2" t="s">
+        <v>142</v>
+      </c>
+      <c r="L2" t="s">
+        <v>143</v>
+      </c>
+      <c r="M2" t="s">
         <v>144</v>
-      </c>
-      <c r="L2" t="s">
-        <v>145</v>
-      </c>
-      <c r="M2" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
@@ -2267,12 +2270,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9234FE1F-FF96-4C35-A780-D38FDA111C06}">
   <dimension ref="A2:L14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L3" sqref="L3:L10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
     <col min="7" max="7" width="14.140625" customWidth="1"/>
     <col min="8" max="8" width="12.5703125" customWidth="1"/>
     <col min="9" max="9" width="14.42578125" customWidth="1"/>
@@ -2281,40 +2286,40 @@
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B2" t="s">
-        <v>156</v>
+        <v>200</v>
       </c>
       <c r="C2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D2" t="s">
-        <v>118</v>
+        <v>194</v>
       </c>
       <c r="E2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F2" t="s">
+        <v>201</v>
+      </c>
+      <c r="G2" t="s">
         <v>120</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>121</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
+        <v>202</v>
+      </c>
+      <c r="J2" t="s">
         <v>122</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>123</v>
       </c>
-      <c r="J2" t="s">
-        <v>124</v>
-      </c>
-      <c r="K2" t="s">
-        <v>125</v>
-      </c>
       <c r="L2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2328,28 +2333,28 @@
         <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>84</v>
+        <v>199</v>
       </c>
       <c r="E3">
         <v>2700</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="I3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="J3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="K3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="L3">
         <f>+unités!K3+unités!L3</f>
@@ -2358,7 +2363,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>73</v>
@@ -2367,28 +2372,28 @@
         <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>84</v>
+        <v>199</v>
       </c>
       <c r="E4">
         <v>2200</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="I4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="K4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="L4">
         <f>+unités!K6+unités!L6+unités!M6</f>
@@ -2397,7 +2402,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>74</v>
@@ -2406,28 +2411,28 @@
         <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>84</v>
+        <v>199</v>
       </c>
       <c r="E5">
         <v>2700</v>
       </c>
       <c r="F5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="J5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="K5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="L5">
         <f>+unités!K7+unités!L7+unités!M7</f>
@@ -2436,7 +2441,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>75</v>
@@ -2445,28 +2450,28 @@
         <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>84</v>
+        <v>199</v>
       </c>
       <c r="E6">
         <v>2200</v>
       </c>
       <c r="F6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="I6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="L6">
         <f>+unités!K8+unités!M8</f>
@@ -2475,7 +2480,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>78</v>
@@ -2484,28 +2489,28 @@
         <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>84</v>
+        <v>199</v>
       </c>
       <c r="E7">
         <v>1500</v>
       </c>
       <c r="F7" t="s">
+        <v>128</v>
+      </c>
+      <c r="G7" t="s">
         <v>130</v>
       </c>
-      <c r="G7" t="s">
-        <v>132</v>
-      </c>
       <c r="H7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="I7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="J7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="K7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="L7">
         <f>+unités!K11+unités!L11+unités!M11</f>
@@ -2514,7 +2519,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B8" s="3">
         <v>201</v>
@@ -2529,22 +2534,22 @@
         <v>1500</v>
       </c>
       <c r="F8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="J8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="K8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="L8">
         <f>+unités!K16+unités!L16+unités!M16</f>
@@ -2553,7 +2558,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B9" s="3">
         <v>203</v>
@@ -2568,22 +2573,22 @@
         <v>900</v>
       </c>
       <c r="F9" t="s">
+        <v>128</v>
+      </c>
+      <c r="G9" t="s">
         <v>130</v>
       </c>
-      <c r="G9" t="s">
-        <v>132</v>
-      </c>
       <c r="H9" t="s">
+        <v>138</v>
+      </c>
+      <c r="I9" t="s">
+        <v>141</v>
+      </c>
+      <c r="J9" t="s">
+        <v>141</v>
+      </c>
+      <c r="K9" t="s">
         <v>140</v>
-      </c>
-      <c r="I9" t="s">
-        <v>143</v>
-      </c>
-      <c r="J9" t="s">
-        <v>143</v>
-      </c>
-      <c r="K9" t="s">
-        <v>142</v>
       </c>
       <c r="L9">
         <f>+unités!K18+unités!M18</f>
@@ -2592,7 +2597,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B10" s="3">
         <v>207</v>
@@ -2607,22 +2612,22 @@
         <v>1200</v>
       </c>
       <c r="F10" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H10" t="s">
+        <v>139</v>
+      </c>
+      <c r="I10" t="s">
         <v>141</v>
       </c>
-      <c r="I10" t="s">
-        <v>143</v>
-      </c>
       <c r="J10" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="K10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="L10">
         <f>+unités!K22+unités!L22</f>
@@ -2660,52 +2665,52 @@
   <sheetData>
     <row r="2" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F2" t="s">
+        <v>156</v>
+      </c>
+      <c r="G2" t="s">
         <v>157</v>
       </c>
-      <c r="C2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>158</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>159</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>160</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>161</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>162</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>163</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>164</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>165</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>166</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s">
         <v>167</v>
-      </c>
-      <c r="P2" t="s">
-        <v>168</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.25">
@@ -2716,10 +2721,10 @@
         <v>19</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="S3">
         <v>2775</v>
@@ -2727,16 +2732,16 @@
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C4" t="s">
         <v>21</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="S4">
         <v>2375</v>
@@ -2744,16 +2749,16 @@
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C5" t="s">
         <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="S5">
         <v>2875</v>
@@ -2761,16 +2766,16 @@
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C6" t="s">
         <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="S6">
         <v>2300</v>
@@ -2778,16 +2783,16 @@
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C7" t="s">
         <v>26</v>
       </c>
       <c r="D7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E7" t="s">
         <v>130</v>
-      </c>
-      <c r="E7" t="s">
-        <v>132</v>
       </c>
       <c r="S7">
         <v>1675</v>
@@ -2795,16 +2800,16 @@
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C8" t="s">
         <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="S8">
         <v>1730</v>
@@ -2812,16 +2817,16 @@
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C9" t="s">
         <v>29</v>
       </c>
       <c r="D9" t="s">
+        <v>128</v>
+      </c>
+      <c r="E9" t="s">
         <v>130</v>
-      </c>
-      <c r="E9" t="s">
-        <v>132</v>
       </c>
       <c r="S9">
         <v>1010</v>
@@ -2829,16 +2834,16 @@
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C10" t="s">
         <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="S10">
         <v>1320</v>
@@ -2867,86 +2872,86 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B6" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D6" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
version avec class paiement débuté
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding\app\inf1163 projet\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C0BF6A-BD4E-44AF-968F-1D1E339711F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20B0462-E358-4C1A-88E7-ED69819FD5C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28365" yWindow="450" windowWidth="21165" windowHeight="13665" activeTab="2" xr2:uid="{42D0C8F0-C429-4306-AA01-3F8905980968}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{42D0C8F0-C429-4306-AA01-3F8905980968}"/>
   </bookViews>
   <sheets>
     <sheet name="locataires" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="205">
   <si>
     <t>prénom</t>
   </si>
@@ -398,9 +398,6 @@
     <t>locataire</t>
   </si>
   <si>
-    <t>date entrée</t>
-  </si>
-  <si>
     <t>date de sortie</t>
   </si>
   <si>
@@ -509,9 +506,6 @@
     <t>idBail</t>
   </si>
   <si>
-    <t>janvier</t>
-  </si>
-  <si>
     <t>février</t>
   </si>
   <si>
@@ -530,9 +524,6 @@
     <t>juillet</t>
   </si>
   <si>
-    <t>août</t>
-  </si>
-  <si>
     <t>septembre</t>
   </si>
   <si>
@@ -648,6 +639,21 @@
   </si>
   <si>
     <t>revouvelabiliter</t>
+  </si>
+  <si>
+    <t>dateEntree</t>
+  </si>
+  <si>
+    <t>dateSortie</t>
+  </si>
+  <si>
+    <t>01/09/2023</t>
+  </si>
+  <si>
+    <t>aout</t>
+  </si>
+  <si>
+    <t>m</t>
   </si>
 </sst>
 </file>
@@ -1052,22 +1058,22 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E2" t="s">
         <v>1</v>
       </c>
       <c r="F2" t="s">
+        <v>189</v>
+      </c>
+      <c r="G2" t="s">
+        <v>190</v>
+      </c>
+      <c r="H2" t="s">
+        <v>191</v>
+      </c>
+      <c r="I2" t="s">
         <v>192</v>
-      </c>
-      <c r="G2" t="s">
-        <v>193</v>
-      </c>
-      <c r="H2" t="s">
-        <v>194</v>
-      </c>
-      <c r="I2" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="3" spans="2:9" ht="16.5" x14ac:dyDescent="0.25">
@@ -1103,7 +1109,7 @@
         <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="F4" t="s">
         <v>48</v>
@@ -1112,7 +1118,7 @@
         <v>61</v>
       </c>
       <c r="H4" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="I4">
         <v>657</v>
@@ -1160,7 +1166,7 @@
         <v>61</v>
       </c>
       <c r="H6" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="I6">
         <v>787</v>
@@ -1184,7 +1190,7 @@
         <v>61</v>
       </c>
       <c r="H7" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="I7">
         <v>763</v>
@@ -1208,7 +1214,7 @@
         <v>61</v>
       </c>
       <c r="H8" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="I8">
         <v>682</v>
@@ -1304,7 +1310,7 @@
         <v>62</v>
       </c>
       <c r="H12" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="I12">
         <v>758</v>
@@ -1313,7 +1319,7 @@
     <row r="13" spans="2:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D13" t="s">
         <v>10</v>
@@ -1328,7 +1334,7 @@
         <v>62</v>
       </c>
       <c r="H13" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="I13">
         <v>718</v>
@@ -1352,7 +1358,7 @@
         <v>62</v>
       </c>
       <c r="H14" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="I14">
         <v>811</v>
@@ -1376,7 +1382,7 @@
         <v>62</v>
       </c>
       <c r="H15" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="I15">
         <v>692</v>
@@ -1391,7 +1397,7 @@
         <v>17</v>
       </c>
       <c r="E16" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F16" t="s">
         <v>59</v>
@@ -1424,7 +1430,7 @@
         <v>62</v>
       </c>
       <c r="H17" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="I17">
         <v>738</v>
@@ -1461,7 +1467,7 @@
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -1488,13 +1494,13 @@
         <v>68</v>
       </c>
       <c r="K2" t="s">
+        <v>141</v>
+      </c>
+      <c r="L2" t="s">
         <v>142</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>143</v>
-      </c>
-      <c r="M2" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
@@ -2270,8 +2276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9234FE1F-FF96-4C35-A780-D38FDA111C06}">
   <dimension ref="A2:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2286,40 +2292,40 @@
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C2" t="s">
         <v>118</v>
       </c>
       <c r="D2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F2" t="s">
+        <v>198</v>
+      </c>
+      <c r="G2" t="s">
+        <v>119</v>
+      </c>
+      <c r="H2" t="s">
+        <v>120</v>
+      </c>
+      <c r="I2" t="s">
+        <v>199</v>
+      </c>
+      <c r="J2" t="s">
+        <v>121</v>
+      </c>
+      <c r="K2" t="s">
+        <v>122</v>
+      </c>
+      <c r="L2" t="s">
         <v>145</v>
-      </c>
-      <c r="F2" t="s">
-        <v>201</v>
-      </c>
-      <c r="G2" t="s">
-        <v>120</v>
-      </c>
-      <c r="H2" t="s">
-        <v>121</v>
-      </c>
-      <c r="I2" t="s">
-        <v>202</v>
-      </c>
-      <c r="J2" t="s">
-        <v>122</v>
-      </c>
-      <c r="K2" t="s">
-        <v>123</v>
-      </c>
-      <c r="L2" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2333,28 +2339,28 @@
         <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E3">
         <v>2700</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>125</v>
-      </c>
       <c r="H3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I3" t="s">
+        <v>139</v>
+      </c>
+      <c r="J3" t="s">
+        <v>139</v>
+      </c>
+      <c r="K3" t="s">
         <v>140</v>
-      </c>
-      <c r="J3" t="s">
-        <v>140</v>
-      </c>
-      <c r="K3" t="s">
-        <v>141</v>
       </c>
       <c r="L3">
         <f>+unités!K3+unités!L3</f>
@@ -2363,7 +2369,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>73</v>
@@ -2372,28 +2378,28 @@
         <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E4">
         <v>2200</v>
       </c>
       <c r="F4" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>125</v>
-      </c>
       <c r="H4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L4">
         <f>+unités!K6+unités!L6+unités!M6</f>
@@ -2402,7 +2408,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>74</v>
@@ -2411,28 +2417,28 @@
         <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E5">
         <v>2700</v>
       </c>
       <c r="F5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L5">
         <f>+unités!K7+unités!L7+unités!M7</f>
@@ -2441,7 +2447,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>75</v>
@@ -2450,28 +2456,28 @@
         <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E6">
         <v>2200</v>
       </c>
       <c r="F6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L6">
         <f>+unités!K8+unités!M8</f>
@@ -2480,7 +2486,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>78</v>
@@ -2489,28 +2495,28 @@
         <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E7">
         <v>1500</v>
       </c>
       <c r="F7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L7">
         <f>+unités!K11+unités!L11+unités!M11</f>
@@ -2519,7 +2525,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B8" s="3">
         <v>201</v>
@@ -2534,22 +2540,22 @@
         <v>1500</v>
       </c>
       <c r="F8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L8">
         <f>+unités!K16+unités!L16+unités!M16</f>
@@ -2558,7 +2564,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B9" s="3">
         <v>203</v>
@@ -2573,22 +2579,22 @@
         <v>900</v>
       </c>
       <c r="F9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L9">
         <f>+unités!K18+unités!M18</f>
@@ -2597,7 +2603,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B10" s="3">
         <v>207</v>
@@ -2612,22 +2618,22 @@
         <v>1200</v>
       </c>
       <c r="F10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H10" t="s">
+        <v>138</v>
+      </c>
+      <c r="I10" t="s">
+        <v>140</v>
+      </c>
+      <c r="J10" t="s">
         <v>139</v>
       </c>
-      <c r="I10" t="s">
-        <v>141</v>
-      </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>140</v>
-      </c>
-      <c r="K10" t="s">
-        <v>141</v>
       </c>
       <c r="L10">
         <f>+unités!K22+unités!L22</f>
@@ -2653,8 +2659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18683229-A73B-42E8-8BF2-829EA24B5669}">
   <dimension ref="B2:S10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2665,52 +2671,52 @@
   <sheetData>
     <row r="2" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C2" t="s">
         <v>118</v>
       </c>
       <c r="D2" t="s">
-        <v>119</v>
+        <v>200</v>
       </c>
       <c r="E2" t="s">
-        <v>120</v>
+        <v>201</v>
       </c>
       <c r="F2" t="s">
+        <v>204</v>
+      </c>
+      <c r="G2" t="s">
+        <v>155</v>
+      </c>
+      <c r="H2" t="s">
         <v>156</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>157</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>158</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>159</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>160</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
+        <v>203</v>
+      </c>
+      <c r="N2" t="s">
         <v>161</v>
       </c>
-      <c r="L2" t="s">
+      <c r="O2" t="s">
         <v>162</v>
       </c>
-      <c r="M2" t="s">
+      <c r="P2" t="s">
         <v>163</v>
       </c>
-      <c r="N2" t="s">
+      <c r="Q2" t="s">
         <v>164</v>
-      </c>
-      <c r="O2" t="s">
-        <v>165</v>
-      </c>
-      <c r="P2" t="s">
-        <v>166</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.25">
@@ -2721,10 +2727,10 @@
         <v>19</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>124</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>125</v>
       </c>
       <c r="S3">
         <v>2775</v>
@@ -2732,16 +2738,16 @@
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C4" t="s">
         <v>21</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>124</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>125</v>
       </c>
       <c r="S4">
         <v>2375</v>
@@ -2749,16 +2755,16 @@
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C5" t="s">
         <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="S5">
         <v>2875</v>
@@ -2766,16 +2772,16 @@
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C6" t="s">
         <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="S6">
         <v>2300</v>
@@ -2783,16 +2789,16 @@
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C7" t="s">
         <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E7" t="s">
-        <v>130</v>
+        <v>202</v>
       </c>
       <c r="S7">
         <v>1675</v>
@@ -2800,16 +2806,16 @@
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C8" t="s">
         <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="S8">
         <v>1730</v>
@@ -2817,16 +2823,16 @@
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C9" t="s">
         <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E9" t="s">
-        <v>130</v>
+        <v>202</v>
       </c>
       <c r="S9">
         <v>1010</v>
@@ -2834,16 +2840,16 @@
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C10" t="s">
         <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="S10">
         <v>1320</v>
@@ -2872,86 +2878,86 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B4" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C4" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D4" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B5" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C5" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D5" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B6" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C6" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D6" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>